<commit_message>
Add psu parameters and loading psu parameters on database
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4DDEB7-BB3F-48AA-80B5-BB2E1D693744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10539BC-8CC0-4782-B38A-50B4D6FE58F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>refComponent</t>
   </si>
@@ -65,9 +65,6 @@
     <t>MPS</t>
   </si>
   <si>
-    <t>PSU1</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -99,6 +96,24 @@
   </si>
   <si>
     <t>0.</t>
+  </si>
+  <si>
+    <t>ref Component</t>
+  </si>
+  <si>
+    <t>equivalence code</t>
+  </si>
+  <si>
+    <t>info jack</t>
+  </si>
+  <si>
+    <t>2,1mm</t>
+  </si>
+  <si>
+    <t>MOSO</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
@@ -418,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,47 +562,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C1A57E-9018-4853-86FB-0FF332F7A899}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>220</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>191498138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -607,40 +646,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1500</v>

</xml_diff>

<commit_message>
Add all Consumer Widget !!
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10539BC-8CC0-4782-B38A-50B4D6FE58F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40738538-91BE-48CB-B134-83E992D9C4DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>refComponent</t>
   </si>
@@ -65,39 +65,15 @@
     <t>MPS</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>voltage_output</t>
   </si>
   <si>
     <t>voltage_input</t>
   </si>
   <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>voltage</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>BCM72180</t>
   </si>
   <si>
-    <t>AVS CORE</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>AVS STB</t>
-  </si>
-  <si>
-    <t>0.</t>
-  </si>
-  <si>
     <t>ref Component</t>
   </si>
   <si>
@@ -114,6 +90,36 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>Wifi</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Soc</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>voltage input</t>
+  </si>
+  <si>
+    <t>current input</t>
+  </si>
+  <si>
+    <t>SKY85207</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Avs Core</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C1A57E-9018-4853-86FB-0FF332F7A899}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +581,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,12 +592,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>191498138</v>
@@ -607,7 +613,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>220</v>
@@ -615,7 +621,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -623,10 +629,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -636,20 +642,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47F608-0CD7-4217-9FA1-5772B3D2AAF8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
@@ -657,35 +666,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4">
+        <v>191477712</v>
+      </c>
+      <c r="C4">
+        <v>191479021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0.8</v>
+      </c>
+      <c r="C5">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
         <v>1500</v>
       </c>
-      <c r="C4">
-        <v>2000</v>
+      <c r="C6">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Function : Add child/parent connection and update parameters for all widgets
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40738538-91BE-48CB-B134-83E992D9C4DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19D8416-1EE5-2F44-838E-C189176B7CB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -439,16 +439,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,7 +476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -504,7 +504,7 @@
         <v>191496767</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -518,7 +518,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -532,7 +532,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -543,10 +543,10 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -574,12 +574,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -587,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -603,7 +603,7 @@
         <v>191498138</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -619,7 +619,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -627,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -644,16 +644,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47F608-0CD7-4217-9FA1-5772B3D2AAF8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -664,7 +664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -675,7 +675,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -686,7 +686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -697,7 +697,7 @@
         <v>191479021</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -708,7 +708,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Feature {Start} : add efficiency formula for DCDC
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D53F91D-2186-4F3C-9D29-B1EA7F8D04F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696378C0-D4E6-284A-9068-82EAAEC0CF22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
     <sheet name="PSU" sheetId="2" r:id="rId2"/>
     <sheet name="CONSUMER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,6 +20,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>refComponent</t>
   </si>
@@ -120,6 +124,14 @@
   </si>
   <si>
     <t>Avs Core</t>
+  </si>
+  <si>
+    <t>Formule calcul rendement
+Vin, Vout, split, f&lt;split, f&gt;split
+séparateur : espace</t>
+  </si>
+  <si>
+    <t>12/5/0,1/-669890*x**4+176938*x**3-16759*x**2+689*x+77/1*x**3-9*x**2+14*x+87</t>
   </si>
 </sst>
 </file>
@@ -155,8 +167,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,18 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="249" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,7 +499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -490,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -504,7 +527,7 @@
         <v>191496767</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -518,7 +541,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -532,7 +555,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -546,7 +569,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -559,6 +582,22 @@
       <c r="D8">
         <v>3.3</v>
       </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,12 +613,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -587,7 +626,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -595,7 +634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -603,7 +642,7 @@
         <v>191498138</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -611,7 +650,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -619,7 +658,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -627,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -648,12 +687,12 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -664,7 +703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -675,7 +714,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -686,7 +725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -697,7 +736,7 @@
         <v>191479021</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -708,7 +747,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Function Efficiency formula update Functional if voltage input and output of DC/DC are identical to the associated formula
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696378C0-D4E6-284A-9068-82EAAEC0CF22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAABC8F-2656-4BAC-BB90-BFDB72F9B5CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
     <sheet name="PSU" sheetId="2" r:id="rId2"/>
     <sheet name="CONSUMER" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,10 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>refComponent</t>
   </si>
@@ -131,7 +127,13 @@
 séparateur : espace</t>
   </si>
   <si>
-    <t>12/5/0,1/-669890*x**4+176938*x**3-16759*x**2+689*x+77/1*x**3-9*x**2+14*x+87</t>
+    <t>12/5/0.1/-669890*x**4+176938*x**3-16759*x**2+689*x+77/1*x**3-9*x**2+14*x+87</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>sdf</t>
   </si>
 </sst>
 </file>
@@ -460,18 +462,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="249" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -513,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -527,7 +529,7 @@
         <v>191496767</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -541,7 +543,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -555,7 +557,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -569,7 +571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -583,7 +585,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -591,11 +593,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
@@ -613,12 +615,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -626,7 +628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -634,7 +636,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -642,7 +644,7 @@
         <v>191498138</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -650,7 +652,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -658,7 +660,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -666,7 +668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -681,18 +683,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47F608-0CD7-4217-9FA1-5772B3D2AAF8}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -702,8 +704,11 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -713,8 +718,11 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -724,8 +732,11 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -735,8 +746,11 @@
       <c r="C4">
         <v>191479021</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -746,8 +760,11 @@
       <c r="C5">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -756,6 +773,9 @@
       </c>
       <c r="C6">
         <v>250</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add file for stylesheet
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAABC8F-2656-4BAC-BB90-BFDB72F9B5CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F11D0CD-61AA-44B5-AD7C-95176C44BCE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -683,10 +683,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A47F608-0CD7-4217-9FA1-5772B3D2AAF8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -708,7 +708,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -722,7 +722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -736,7 +736,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -750,7 +750,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -764,7 +764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -776,6 +776,12 @@
       </c>
       <c r="D6">
         <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f>1*0.2^3-9*0.2^2+14*0.2+87</f>
+        <v>89.448000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DCDC : add "Mode"
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B905C15B-9172-441D-8308-8CD472053AE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCE116C-620B-4BB1-9AF1-BE378931B91E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,68 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D3896D1E-7627-4052-8237-9F53D35C22B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pulse frequency modulation
+Forced PWM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{D8BAF521-560E-44F4-9C0A-C67EF7A67DFC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Vin, Vout, split, f&lt;split, f&gt;split
+Séparateur : /</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>supplier</t>
   </si>
@@ -76,23 +136,12 @@
     <t>UK</t>
   </si>
   <si>
-    <t>Formule calcul rendement
-Vin, Vout, split, f&lt;split, f&gt;split
-séparateur : espace</t>
-  </si>
-  <si>
     <t>12/5/0.1/-669890*x**4+176938*x**3-16759*x**2+689*x+77/1*x**3-9*x**2+14*x+87</t>
   </si>
   <si>
     <t>current Max</t>
   </si>
   <si>
-    <t>Vin, Vout, split, f&lt;split, f&gt;split</t>
-  </si>
-  <si>
-    <t>séparateur : espace</t>
-  </si>
-  <si>
     <t>Rendement</t>
   </si>
   <si>
@@ -109,13 +158,19 @@
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Pulse Frequency Mod.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +185,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -448,11 +516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,46 +528,50 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" customWidth="1"/>
-    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -512,26 +584,26 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
         <v>191422423</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4.2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>18</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.8</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -544,23 +616,23 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
         <v>191345519</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4.2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5</v>
-      </c>
-      <c r="M3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -573,28 +645,29 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
         <v>191496767</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>5.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3.3</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -607,6 +680,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -614,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C1A57E-9018-4853-86FB-0FF332F7A899}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New Function : Add PMIC component
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CE541F-BFDF-4B71-BA02-8C89ED38317B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2127ECB-5B83-4A7B-B155-B7F427E9FCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
-    <sheet name="PSU" sheetId="2" r:id="rId2"/>
-    <sheet name="LDO" sheetId="3" r:id="rId3"/>
-    <sheet name="SWITCH" sheetId="4" r:id="rId4"/>
+    <sheet name="PMIC" sheetId="5" r:id="rId2"/>
+    <sheet name="PSU" sheetId="2" r:id="rId3"/>
+    <sheet name="LDO" sheetId="3" r:id="rId4"/>
+    <sheet name="SWITCH" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
   <si>
     <t>supplier</t>
   </si>
@@ -96,12 +97,6 @@
     <t>currentMax</t>
   </si>
   <si>
-    <t>voltageOutputRangeMin</t>
-  </si>
-  <si>
-    <t>voltageOutputRangeMax</t>
-  </si>
-  <si>
     <t>MP1652</t>
   </si>
   <si>
@@ -238,13 +233,124 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Voltage Input Range Min</t>
+  </si>
+  <si>
+    <t>Voltage Input Range Max</t>
+  </si>
+  <si>
+    <t>Voltage Output Range Min</t>
+  </si>
+  <si>
+    <t>Voltage Output Range Max</t>
+  </si>
+  <si>
+    <t>Equivalence Code</t>
+  </si>
+  <si>
+    <t>Feedback voltage</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>SOT563</t>
+  </si>
+  <si>
+    <t>MP1654</t>
+  </si>
+  <si>
+    <t>Forced PWM</t>
+  </si>
+  <si>
+    <t>MP1652C</t>
+  </si>
+  <si>
+    <t>MP1653C</t>
+  </si>
+  <si>
+    <t>MP1601</t>
+  </si>
+  <si>
+    <t>MP1605</t>
+  </si>
+  <si>
+    <t>MP1605C</t>
+  </si>
+  <si>
+    <t>MP1601A</t>
+  </si>
+  <si>
+    <t>MP2331</t>
+  </si>
+  <si>
+    <t>MP2330</t>
+  </si>
+  <si>
+    <t>SOT583</t>
+  </si>
+  <si>
+    <t>BCM59400</t>
+  </si>
+  <si>
+    <t>Broadcom</t>
+  </si>
+  <si>
+    <t>DCDC or LDO</t>
+  </si>
+  <si>
+    <t>DCDC</t>
+  </si>
+  <si>
+    <t>Current Max</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>0V8_AVS_STB</t>
+  </si>
+  <si>
+    <t>0V95_AVS_CPU</t>
+  </si>
+  <si>
+    <t>D0V8-A0V8</t>
+  </si>
+  <si>
+    <t>D1V8-A1V8</t>
+  </si>
+  <si>
+    <t>D3V3-A3V3</t>
+  </si>
+  <si>
+    <t>AON_3V3</t>
+  </si>
+  <si>
+    <t>AON_0V8</t>
+  </si>
+  <si>
+    <t>1V8_LPDDR4</t>
+  </si>
+  <si>
+    <t>AON_1V8</t>
+  </si>
+  <si>
+    <t>0V6_LPDDR4</t>
+  </si>
+  <si>
+    <t>1V1_LPDDR4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,13 +387,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -302,17 +420,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -323,6 +432,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,165 +748,843 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="36.140625" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" customWidth="1"/>
+    <col min="11" max="11" width="12" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="10" customWidth="1"/>
     <col min="13" max="13" width="6.140625" customWidth="1"/>
     <col min="14" max="14" width="5.28515625" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>4</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E2" s="12">
+        <v>191422415</v>
+      </c>
+      <c r="F2" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G2" s="12">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H2" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="12">
+        <v>17</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="12">
+        <v>3</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="12">
+        <v>191345519</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G3" s="12">
+        <v>17</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I3" s="12">
+        <v>17</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="15">
+        <v>191469070</v>
+      </c>
+      <c r="F4" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>17</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="12">
+        <v>17</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="15">
+        <v>191422423</v>
+      </c>
+      <c r="F5" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="12">
+        <v>18</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="12">
+        <v>18</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="12">
+        <v>191469046</v>
+      </c>
+      <c r="F6" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G6" s="12">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="12">
+        <v>18</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>3</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="12">
+        <v>191496767</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I7" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="12">
+        <v>191689825</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I8" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="12">
+        <v>191640964</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G9" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I9" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="12">
+        <v>191639458</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G10" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I10" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="12">
+        <v>191495520</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I11" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="G12" s="12">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H12" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="12">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J12" s="12"/>
+      <c r="K12" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>191422423</v>
-      </c>
-      <c r="F2">
+      <c r="D13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="12">
         <v>4.2</v>
       </c>
-      <c r="G2">
-        <v>18</v>
-      </c>
-      <c r="H2">
+      <c r="G13" s="12">
+        <v>24</v>
+      </c>
+      <c r="H13" s="12">
         <v>0.8</v>
       </c>
-      <c r="I2">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3">
-        <v>191345519</v>
-      </c>
-      <c r="F3">
-        <v>4.2</v>
-      </c>
-      <c r="G3">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4">
-        <v>191496767</v>
-      </c>
-      <c r="F4">
-        <v>2.5</v>
-      </c>
-      <c r="G4">
-        <v>5.5</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="I13" s="12">
+        <v>21</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -772,6 +1594,479 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FB9125-F5C6-4552-A4A1-D0888055A02D}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="13">
+        <v>75</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="12">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12">
+        <v>5</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="J3" s="13">
+        <v>75</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="12">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>5</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="13">
+        <v>75</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="12">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="J5" s="13">
+        <v>75</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="12">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="I6" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J6" s="13">
+        <v>75</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="12">
+        <v>5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="I7" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="J7" s="13">
+        <v>75</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>5</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="J8" s="13">
+        <v>16</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5</v>
+      </c>
+      <c r="G9" s="12">
+        <v>5</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="J9" s="13">
+        <v>36</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>5</v>
+      </c>
+      <c r="G10" s="12">
+        <v>5</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="J10" s="13">
+        <v>36</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="17"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="J11" s="13">
+        <v>75</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="12">
+        <v>191478040</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="12">
+        <v>5</v>
+      </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I12" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J12" s="13">
+        <v>75</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C1A57E-9018-4853-86FB-0FF332F7A899}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -790,33 +2085,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>191498138</v>
@@ -831,7 +2126,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +2134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD98151-495C-4244-B363-DD15384BDD8A}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -860,41 +2155,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="4"/>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>0.3</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>1.4</v>
@@ -908,10 +2203,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0.3</v>
@@ -931,10 +2226,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>0.3</v>
@@ -957,12 +2252,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83E2B1A-1A60-4C00-82BC-6720B8BC26B3}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,40 +2272,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -1019,24 +2314,24 @@
         <v>0.08</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="6">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3">
         <v>191474787</v>
       </c>
-      <c r="G2" s="7">
-        <v>5</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1045,24 +2340,24 @@
         <v>0.08</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="6">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3">
         <v>191475792</v>
       </c>
-      <c r="G3" s="7">
-        <v>5</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0.15</v>
@@ -1071,10 +2366,10 @@
         <v>0.4</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <v>191285953</v>
@@ -1088,7 +2383,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1097,10 +2392,10 @@
         <v>0.06</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>191255570</v>
@@ -1114,7 +2409,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1123,10 +2418,10 @@
         <v>0.02</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>191478917</v>
@@ -1146,7 +2441,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Function : Move view from the scene && move an widget from the scene
</commit_message>
<xml_diff>
--- a/DATA_BASE.xlsx
+++ b/DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2127ECB-5B83-4A7B-B155-B7F427E9FCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC585B4-30D2-49DD-B534-5CA09090DC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="35835" windowHeight="20220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCDC" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Auteur:</t>
         </r>
@@ -51,7 +51,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Pulse frequency modulation
@@ -67,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Auteur:</t>
         </r>
@@ -76,7 +76,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Vin, Vout, split, f&lt;split, f&gt;split
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
   <si>
     <t>supplier</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>RICOH</t>
-  </si>
-  <si>
-    <t>20220302-03</t>
   </si>
   <si>
     <t>voltageOutput</t>
@@ -370,14 +367,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -751,7 +748,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,33 +784,33 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>5</v>
@@ -844,7 +841,7 @@
         <v>0.8</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -885,7 +882,7 @@
         <v>0.8</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -895,7 +892,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>5</v>
@@ -904,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="15">
         <v>191469070</v>
@@ -926,7 +923,7 @@
         <v>0.8</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -969,7 +966,7 @@
         <v>0.8</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -979,7 +976,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>5</v>
@@ -988,7 +985,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="12">
         <v>191469046</v>
@@ -1010,7 +1007,7 @@
         <v>0.8</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -1051,7 +1048,7 @@
         <v>0.6</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -1061,7 +1058,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>5</v>
@@ -1092,7 +1089,7 @@
         <v>0.6</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -1102,7 +1099,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>5</v>
@@ -1111,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="12">
         <v>191640964</v>
@@ -1133,7 +1130,7 @@
         <v>0.6</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1143,7 +1140,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>5</v>
@@ -1174,7 +1171,7 @@
         <v>0.6</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -1184,7 +1181,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>5</v>
@@ -1193,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="12">
         <v>191495520</v>
@@ -1215,7 +1212,7 @@
         <v>0.6</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -1225,7 +1222,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>5</v>
@@ -1237,7 +1234,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="12">
         <v>4.2</v>
@@ -1256,7 +1253,7 @@
         <v>0.8</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -1266,7 +1263,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>5</v>
@@ -1278,7 +1275,7 @@
         <v>23</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="12">
         <v>4.2</v>
@@ -1297,7 +1294,7 @@
         <v>0.8</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
@@ -1597,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FB9125-F5C6-4552-A4A1-D0888055A02D}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,46 +1620,46 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C2" s="12">
         <v>191478040</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="12">
         <v>3</v>
@@ -1683,22 +1680,22 @@
         <v>75</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C3" s="12">
         <v>191478040</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="12">
         <v>3</v>
@@ -1719,22 +1716,22 @@
         <v>75</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C4" s="12">
         <v>191478040</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="12">
         <v>1.5</v>
@@ -1755,22 +1752,22 @@
         <v>75</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L4" s="17"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C5" s="12">
         <v>191478040</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="12">
         <v>1.5</v>
@@ -1791,22 +1788,22 @@
         <v>75</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L5" s="17"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C6" s="12">
         <v>191478040</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="12">
         <v>1.5</v>
@@ -1827,22 +1824,22 @@
         <v>75</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="17"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C7" s="12">
         <v>191478040</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="12">
         <v>1.5</v>
@@ -1863,22 +1860,22 @@
         <v>75</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C8" s="12">
         <v>191478040</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="12">
         <v>0.1</v>
@@ -1899,22 +1896,22 @@
         <v>16</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C9" s="12">
         <v>191478040</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="12">
         <v>0.1</v>
@@ -1935,22 +1932,22 @@
         <v>36</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C10" s="12">
         <v>191478040</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="17">
         <v>0.1</v>
@@ -1971,22 +1968,22 @@
         <v>36</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L10" s="17"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C11" s="12">
         <v>191478040</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="12">
         <v>1.5</v>
@@ -2007,22 +2004,22 @@
         <v>75</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="C12" s="12">
         <v>191478040</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="12">
         <v>1.5</v>
@@ -2043,7 +2040,7 @@
         <v>75</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L12" s="17"/>
     </row>
@@ -2138,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD98151-495C-4244-B363-DD15384BDD8A}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,7 +2171,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2188,8 +2185,8 @@
       <c r="C2">
         <v>0.3</v>
       </c>
-      <c r="D2" t="s">
-        <v>26</v>
+      <c r="D2">
+        <v>191693994</v>
       </c>
       <c r="E2">
         <v>1.4</v>
@@ -2198,12 +2195,12 @@
         <v>5.25</v>
       </c>
       <c r="G2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -2212,7 +2209,7 @@
         <v>0.3</v>
       </c>
       <c r="D3">
-        <v>256452</v>
+        <v>191694800</v>
       </c>
       <c r="E3">
         <v>1.4</v>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -2273,13 +2270,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>8</v>
@@ -2291,21 +2288,21 @@
         <v>9</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -2314,10 +2311,10 @@
         <v>0.08</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="3">
         <v>191474787</v>
@@ -2331,7 +2328,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2340,10 +2337,10 @@
         <v>0.08</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3">
         <v>191475792</v>
@@ -2357,7 +2354,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>0.15</v>
@@ -2366,10 +2363,10 @@
         <v>0.4</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>191285953</v>
@@ -2383,7 +2380,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2392,10 +2389,10 @@
         <v>0.06</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>191255570</v>
@@ -2409,7 +2406,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -2418,10 +2415,10 @@
         <v>0.02</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6">
         <v>191478917</v>
@@ -2441,7 +2438,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>